<commit_message>
2 - Implémentation du parsing du fichier et mappage en Participant
</commit_message>
<xml_diff>
--- a/src/test/resources/Participants.xlsx
+++ b/src/test/resources/Participants.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbarthez\SOFTWAY MEDICAL\Softway Developer Day - Documents\General\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace_sdd\SDD\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="604" documentId="8_{447FF050-A089-4AC3-89AD-B74CD73EC517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7A8AED43-1389-472E-9DEC-703763941158}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D873C7E-E1AE-4B6F-8FE9-D4989437636B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31440" yWindow="675" windowWidth="21600" windowHeight="13350" xr2:uid="{B1BA483A-1E2F-4E5A-B2B3-BB33C7328C77}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B1BA483A-1E2F-4E5A-B2B3-BB33C7328C77}"/>
   </bookViews>
   <sheets>
     <sheet name="Participants" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -552,7 +552,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -607,9 +607,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,7 +626,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -925,13 +922,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BA45B4-BC64-4B4B-A26A-78494D54C601}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:XFD115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
@@ -940,7 +937,7 @@
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -964,7 +961,7 @@
       </c>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -987,7 +984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1010,7 +1007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19.5" customHeight="1">
+    <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1033,7 +1030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1056,7 +1053,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1079,7 +1076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1102,7 +1099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1125,7 +1122,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1148,7 +1145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1194,7 +1191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1217,7 +1214,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1240,7 +1237,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -1263,7 +1260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1309,7 +1306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1332,7 +1329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -1355,7 +1352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -1378,7 +1375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
@@ -1401,7 +1398,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -1424,7 +1421,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -1447,7 +1444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -1470,7 +1467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>73</v>
       </c>
@@ -1493,7 +1490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
@@ -1539,7 +1536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>79</v>
       </c>
@@ -1562,7 +1559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -1585,7 +1582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
@@ -1608,7 +1605,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>83</v>
       </c>
@@ -1631,7 +1628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>86</v>
       </c>
@@ -1654,7 +1651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>89</v>
       </c>
@@ -1677,7 +1674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
@@ -1700,7 +1697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>93</v>
       </c>
@@ -1723,7 +1720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>95</v>
       </c>
@@ -1746,7 +1743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>97</v>
       </c>
@@ -1769,7 +1766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>100</v>
       </c>
@@ -1792,7 +1789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>102</v>
       </c>
@@ -1815,7 +1812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>104</v>
       </c>
@@ -1838,7 +1835,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>106</v>
       </c>
@@ -1861,7 +1858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16.5" customHeight="1">
+    <row r="41" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>108</v>
       </c>
@@ -1884,7 +1881,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>110</v>
       </c>
@@ -1907,7 +1904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>112</v>
       </c>
@@ -1930,7 +1927,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>114</v>
       </c>
@@ -1953,7 +1950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>116</v>
       </c>
@@ -1976,7 +1973,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>117</v>
       </c>
@@ -1999,7 +1996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>119</v>
       </c>
@@ -2022,7 +2019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>121</v>
       </c>
@@ -2045,7 +2042,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>123</v>
       </c>
@@ -2068,7 +2065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>125</v>
       </c>
@@ -2091,7 +2088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>127</v>
       </c>
@@ -2114,7 +2111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>129</v>
       </c>
@@ -2137,7 +2134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>131</v>
       </c>
@@ -2160,7 +2157,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>133</v>
       </c>
@@ -2183,7 +2180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>135</v>
       </c>
@@ -2206,7 +2203,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>137</v>
       </c>
@@ -2229,7 +2226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>139</v>
       </c>
@@ -2252,7 +2249,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>141</v>
       </c>
@@ -2275,7 +2272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
@@ -2298,7 +2295,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>145</v>
       </c>
@@ -2321,7 +2318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>146</v>
       </c>
@@ -2344,7 +2341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>148</v>
       </c>
@@ -2367,7 +2364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>150</v>
       </c>
@@ -2390,7 +2387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>151</v>
       </c>
@@ -2413,7 +2410,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>153</v>
       </c>
@@ -2436,7 +2433,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>154</v>
       </c>
@@ -2459,7 +2456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>155</v>
       </c>
@@ -2482,7 +2479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>157</v>
       </c>
@@ -2505,7 +2502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>158</v>
       </c>
@@ -2528,7 +2525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>160</v>
       </c>
@@ -2551,7 +2548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>162</v>
       </c>
@@ -2574,7 +2571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>164</v>
       </c>
@@ -2597,7 +2594,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>167</v>
       </c>
@@ -2620,7 +2617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>169</v>
       </c>
@@ -2643,50 +2640,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="E75" s="5"/>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="E76" s="5"/>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="E77" s="5"/>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="E79" s="5"/>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="E80" s="5"/>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="E81" s="5"/>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="5"/>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="5"/>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="E84" s="5"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H84">
-    <sortCondition ref="A2:A84"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H74">
+    <sortCondition ref="A2:A74"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E82:E83 E2:E73" xr:uid="{DA134F2B-EA5F-42CD-8EA6-5DCFECFDAED5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E73" xr:uid="{DA134F2B-EA5F-42CD-8EA6-5DCFECFDAED5}">
       <formula1>"OUI,NON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2695,12 +2654,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2818,19 +2774,43 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D777B8FD-83DC-4D65-8CA0-C4F21085F961}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7489D0B0-3340-4493-8A73-ED36DA0467BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEF12E5B-6750-48BA-A46C-31A7D76892DC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEF12E5B-6750-48BA-A46C-31A7D76892DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7489D0B0-3340-4493-8A73-ED36DA0467BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D777B8FD-83DC-4D65-8CA0-C4F21085F961}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>